<commit_message>
Updated efuels + ammonia input databases
Numbers not accurate yet, just form!
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F294832-F4FB-4597-8F93-EADD17FBF52E}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2E42E8E-BC70-4891-85BD-0F04F6277FFF}"/>
   <bookViews>
-    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-20835" yWindow="-19260" windowWidth="22860" windowHeight="18315" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="Storages" sheetId="3" r:id="rId3"/>
     <sheet name="DropDown" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="CIQWBGuid" hidden="1">"9e92b299-41ef-42cf-ac4c-11a4ddc4cf09"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
@@ -76,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>Unit</t>
   </si>
@@ -123,9 +120,6 @@
     <t>Cap_Output2_max</t>
   </si>
   <si>
-    <t>Cap_Output_1_max</t>
-  </si>
-  <si>
     <t>Connection</t>
   </si>
   <si>
@@ -213,129 +207,48 @@
     <t>Object_type</t>
   </si>
   <si>
-    <t>storage_investment_tech_lifetime</t>
-  </si>
-  <si>
-    <t>number_of_storages</t>
-  </si>
-  <si>
-    <t>storage_investment_cost</t>
-  </si>
-  <si>
     <t>connection_investment_tech_lifetime</t>
   </si>
   <si>
-    <t>number_of_connections</t>
-  </si>
-  <si>
     <t>mean_efficiency</t>
   </si>
   <si>
     <t>units_on_cost</t>
   </si>
   <si>
-    <t>minimum_op_point</t>
-  </si>
-  <si>
-    <t>unit_idle_heat_rate</t>
-  </si>
-  <si>
     <t>resolution_output</t>
   </si>
   <si>
     <t>demand</t>
   </si>
   <si>
-    <t>unit_investment_variable_type</t>
-  </si>
-  <si>
-    <t>unit_investment_tech_lifetime</t>
-  </si>
-  <si>
-    <t>number_of_units</t>
-  </si>
-  <si>
-    <t>Error messages:</t>
-  </si>
-  <si>
     <t>object_type</t>
   </si>
   <si>
     <t>PV_plant</t>
   </si>
   <si>
-    <t>Solar_Plant_Kasso</t>
-  </si>
-  <si>
-    <t>Power_Kasso</t>
-  </si>
-  <si>
-    <t>unit_investment_variable_type_continuous</t>
-  </si>
-  <si>
-    <t>35Y</t>
-  </si>
-  <si>
-    <t>Electrolyzer</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>Hydrogen_Kasso</t>
-  </si>
-  <si>
-    <t>Waste_Heat</t>
-  </si>
-  <si>
-    <t>25Y</t>
-  </si>
-  <si>
-    <t>Steam_Plant</t>
-  </si>
-  <si>
     <t>Electric_Steam_Boiler</t>
   </si>
   <si>
-    <t>Steam</t>
-  </si>
-  <si>
-    <t>20Y</t>
-  </si>
-  <si>
-    <t>Hydrogen_storage_Kasso</t>
-  </si>
-  <si>
     <t>Hydrogen_storage</t>
   </si>
   <si>
     <t>fix_node_state</t>
   </si>
   <si>
-    <t>Ammonia_storage_Kasso</t>
-  </si>
-  <si>
     <t>Ammonia_storage</t>
   </si>
   <si>
-    <t>power_line_Wholesale_Kasso</t>
-  </si>
-  <si>
     <t>Power_line</t>
   </si>
   <si>
-    <t>Power_Wholesale</t>
-  </si>
-  <si>
     <t>connection_type_lossless_bidirectional</t>
   </si>
   <si>
     <t>40Y</t>
   </si>
   <si>
-    <t>pipeline_storage_hydrogen</t>
-  </si>
-  <si>
     <t>Hydrogen_pipeline</t>
   </si>
   <si>
@@ -345,33 +258,9 @@
     <t>50Y</t>
   </si>
   <si>
-    <t>pipeline_District_Heating</t>
-  </si>
-  <si>
     <t>Heat_pipeline</t>
   </si>
   <si>
-    <t>District_Heating</t>
-  </si>
-  <si>
-    <t>pipeline_storage_ammonia</t>
-  </si>
-  <si>
-    <t>Ammonia_Kasso</t>
-  </si>
-  <si>
-    <t>ASU</t>
-  </si>
-  <si>
-    <t>Ammonia_synthezyser</t>
-  </si>
-  <si>
-    <t>Nitrogen</t>
-  </si>
-  <si>
-    <t>Ammonia</t>
-  </si>
-  <si>
     <t>Ammonia_pipeline</t>
   </si>
   <si>
@@ -391,13 +280,100 @@
   </si>
   <si>
     <t>Haber_Bosch_reactor</t>
+  </si>
+  <si>
+    <t>start_up_cost</t>
+  </si>
+  <si>
+    <t>shut_down_cost</t>
+  </si>
+  <si>
+    <t>minimum_op_point_Input1</t>
+  </si>
+  <si>
+    <t>minimum_op_point_Input2</t>
+  </si>
+  <si>
+    <t>minimum_op_point_Output1</t>
+  </si>
+  <si>
+    <t>minimum_op_point_Output2</t>
+  </si>
+  <si>
+    <t>solar_plant</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>electrolyzer</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>steam</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>steam_plant</t>
+  </si>
+  <si>
+    <t>initial_connections_invested_available</t>
+  </si>
+  <si>
+    <t>pl_wholesale</t>
+  </si>
+  <si>
+    <t>power_wholesale</t>
+  </si>
+  <si>
+    <t>pl_h2_st</t>
+  </si>
+  <si>
+    <t>h2_st</t>
+  </si>
+  <si>
+    <t>pl_dh</t>
+  </si>
+  <si>
+    <t>dh</t>
+  </si>
+  <si>
+    <t>asu</t>
+  </si>
+  <si>
+    <t>n2</t>
+  </si>
+  <si>
+    <t>nh3</t>
+  </si>
+  <si>
+    <t>nh3_synthesizer</t>
+  </si>
+  <si>
+    <t>pl_nh3_st</t>
+  </si>
+  <si>
+    <t>nh3_st</t>
+  </si>
+  <si>
+    <t>initial_storages_invested</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,24 +386,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -450,19 +408,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -473,6 +431,12 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -490,130 +454,91 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Units"/>
-      <sheetName val="Connections"/>
-      <sheetName val="Storages"/>
-      <sheetName val="Drop_Down"/>
-      <sheetName val="Model_Data_Base (2)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AQ6" totalsRowShown="0">
-  <autoFilter ref="A1:AQ6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="43">
-    <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
-    <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Object_type"/>
-    <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input1"/>
-    <tableColumn id="4" xr3:uid="{C03E717E-B39B-450F-A07B-8C087AA65297}" name="Input2"/>
-    <tableColumn id="5" xr3:uid="{1193D369-BC65-45A6-8749-4CD88E2C1722}" name="Output1"/>
-    <tableColumn id="6" xr3:uid="{4AAC878F-692F-4277-A013-661DCC5DAE26}" name="Output2"/>
-    <tableColumn id="7" xr3:uid="{C21757F9-61E8-45D7-ADA3-80D8624CAEF0}" name="Cap_Input1_existing"/>
-    <tableColumn id="14" xr3:uid="{23796EE3-B67D-45AE-9553-CC3081EFDF57}" name="Cap_Input1_max"/>
-    <tableColumn id="15" xr3:uid="{DF0C0799-CA68-4E9B-A1FB-41F4996C01A9}" name="Cap_Input2_existing"/>
-    <tableColumn id="16" xr3:uid="{8A84DF9A-0F8E-4DA8-A009-F41EF2B05A60}" name="Cap_Input2_max"/>
-    <tableColumn id="17" xr3:uid="{6408F114-841E-472E-92F5-7B63FF1B66F4}" name="Cap_Output1_existing"/>
-    <tableColumn id="18" xr3:uid="{541C17F0-C020-47FE-9DA4-DB76D7416668}" name="Cap_Output_1_max"/>
-    <tableColumn id="19" xr3:uid="{D6FEE63D-DC89-4D1A-9708-5E7C70FD5793}" name="Cap_Output2_existing"/>
-    <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="Cap_Output2_max"/>
-    <tableColumn id="26" xr3:uid="{D0F85E7B-D704-45A0-BE99-26E3A1F08634}" name="mean_efficiency"/>
-    <tableColumn id="28" xr3:uid="{EBC4610B-47F0-44E3-8543-664851FC473C}" name="min_down_time"/>
-    <tableColumn id="27" xr3:uid="{DC89C4F2-3857-45F2-B4A0-642F9C1613A6}" name="ramp_up_Output1"/>
-    <tableColumn id="29" xr3:uid="{5A66563E-85FF-4FFA-9DB7-EAC64F37E721}" name="ramp_up_Output2"/>
-    <tableColumn id="30" xr3:uid="{98C94D50-387A-4596-96E7-17395B3AF62E}" name="ramp_down_Output1"/>
-    <tableColumn id="31" xr3:uid="{FF26E17F-A633-477F-A8B8-3FD0C0B88F7D}" name="ramp_down_Output2"/>
-    <tableColumn id="32" xr3:uid="{D45EEC70-4FBC-44FF-9E9A-E2D38C52BF94}" name="start_up_Output1"/>
-    <tableColumn id="33" xr3:uid="{D8C88D78-E68F-45EF-8A97-7C1F84821946}" name="start_up_Output2"/>
-    <tableColumn id="9" xr3:uid="{50F936EF-D32C-4938-8FCA-291A6A3E82E6}" name="shut_down_Output1"/>
-    <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="shut_down_Output2"/>
-    <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_In_In"/>
-    <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Relation_In_Out"/>
-    <tableColumn id="25" xr3:uid="{95F69D80-80E7-42BD-B42F-59F3C3DC485B}" name="Relation_Out_Out"/>
-    <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="Cost_invest" dataDxfId="2">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Cap_Output1_existing]]*0.56</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="24" xr3:uid="{4D171E04-3F62-4131-BD43-B8A8D03B8530}" name="units_on_cost"/>
-    <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="fom_cost"/>
-    <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost"/>
-    <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Input1"/>
-    <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Input2"/>
-    <tableColumn id="34" xr3:uid="{07BFD460-8B2F-4C66-8709-DAF17E5F2C62}" name="vom_cost_Output1"/>
-    <tableColumn id="35" xr3:uid="{EF2A3F17-0D1A-480E-A13D-A5808719A3ED}" name="vom_cost_Output2"/>
-    <tableColumn id="36" xr3:uid="{CFFB3FD3-3581-4635-8E26-A397976C50BA}" name="minimum_op_point"/>
-    <tableColumn id="37" xr3:uid="{FF4178F5-A47B-4920-A52E-1B3F85F074B2}" name="unit_idle_heat_rate"/>
-    <tableColumn id="38" xr3:uid="{025B798B-AEA0-4557-A1C1-691EF0E57AB5}" name="resolution_output"/>
-    <tableColumn id="39" xr3:uid="{35A52A69-E8FB-4298-8F4F-F2BB77F81158}" name="demand"/>
-    <tableColumn id="40" xr3:uid="{13D3F1BD-DB2E-4B88-B660-2F6A81616F69}" name="unit_investment_variable_type"/>
-    <tableColumn id="41" xr3:uid="{8CF0CBE3-C92A-4542-8737-317CCD5CF213}" name="unit_investment_tech_lifetime"/>
-    <tableColumn id="42" xr3:uid="{363D0C55-B2E1-44C7-87B7-7505E7326FF0}" name="number_of_units"/>
-    <tableColumn id="43" xr3:uid="{D9CDEEFF-E080-4B8B-8CB3-8D91FD4E3834}" name="Error messages:"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}" name="Table16" displayName="Table16" ref="A1:AI6" totalsRowShown="0">
+  <autoFilter ref="A1:AI6" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}"/>
+  <tableColumns count="35">
+    <tableColumn id="1" xr3:uid="{7D298EC1-7302-405B-8F92-0542D7D7F128}" name="Unit"/>
+    <tableColumn id="40" xr3:uid="{DCBF9D29-057B-4317-8290-D82D5B7920ED}" name="Object_type"/>
+    <tableColumn id="2" xr3:uid="{D57D27A7-B5BF-44EE-97E6-A45E663C9B11}" name="Input1"/>
+    <tableColumn id="3" xr3:uid="{DD3DCF60-A9F6-4EAA-9D24-0F3FD89C7DEC}" name="Input2"/>
+    <tableColumn id="4" xr3:uid="{49C08C48-AB3A-4CEA-967C-339B04AB2745}" name="Output1"/>
+    <tableColumn id="5" xr3:uid="{46348012-61C3-43AA-8F2D-1BC64A7CE705}" name="Output2"/>
+    <tableColumn id="35" xr3:uid="{94FDE9A5-447F-4B57-BBC2-02E504C247C8}" name="mean_efficiency"/>
+    <tableColumn id="8" xr3:uid="{A3B55077-666A-4BFB-8509-BB8A1A676249}" name="min_down_time"/>
+    <tableColumn id="26" xr3:uid="{5009ED1F-D49F-4805-8848-5659834445DF}" name="ramp_up_Output1"/>
+    <tableColumn id="28" xr3:uid="{64FF8714-B954-4EC7-B09F-69C76804ABD0}" name="ramp_up_Output2"/>
+    <tableColumn id="27" xr3:uid="{AD053AFC-1F17-4A84-A299-70E506D26F9E}" name="ramp_down_Output1"/>
+    <tableColumn id="29" xr3:uid="{75A0A685-3C3D-474F-BE0A-28D455797398}" name="ramp_down_Output2"/>
+    <tableColumn id="30" xr3:uid="{2A66C5C3-F801-46C1-BD01-247C8C4B1D08}" name="start_up_Output1"/>
+    <tableColumn id="31" xr3:uid="{1FBA8DD4-61E6-4423-AD9A-0CB06E974DD0}" name="start_up_Output2"/>
+    <tableColumn id="32" xr3:uid="{68E91A4E-B79C-430E-A022-77DFEE5CAB98}" name="shut_down_Output1"/>
+    <tableColumn id="33" xr3:uid="{FFECA6E3-22AA-4957-B61D-DFFF43863948}" name="shut_down_Output2"/>
+    <tableColumn id="36" xr3:uid="{46BE177F-7CE9-433F-821C-70EFC44B95B9}" name="start_up_cost"/>
+    <tableColumn id="37" xr3:uid="{23ECD243-879D-4D26-8CC4-DE08EE59A53C}" name="shut_down_cost"/>
+    <tableColumn id="9" xr3:uid="{7094586D-F569-42E6-9659-BFA01BFADAC8}" name="Relation_In_In"/>
+    <tableColumn id="20" xr3:uid="{147C72B7-620D-4714-87E9-E7CB6F571574}" name="Relation_In_Out"/>
+    <tableColumn id="10" xr3:uid="{E3C2CD93-F547-4D58-8A39-A1C9F02F97A8}" name="Relation_Out_Out"/>
+    <tableColumn id="11" xr3:uid="{2EC6318E-BECE-45C0-8327-D7AFF840871E}" name="Cost_invest"/>
+    <tableColumn id="25" xr3:uid="{9F049A47-0213-4397-848B-1EF1B3A45E7A}" name="units_on_cost"/>
+    <tableColumn id="12" xr3:uid="{C4243E50-4545-43FB-A14B-E5CD366C40F9}" name="fom_cost"/>
+    <tableColumn id="24" xr3:uid="{2887EEF0-F5F4-42D9-AF95-2AE9F59DB77A}" name="vom_cost"/>
+    <tableColumn id="13" xr3:uid="{DC6BC9D3-04A9-4083-9F39-97FE2D6E1E50}" name="vom_cost_Input1"/>
+    <tableColumn id="21" xr3:uid="{26064220-D150-4C40-81D6-F230A2D58BBF}" name="vom_cost_Input2"/>
+    <tableColumn id="22" xr3:uid="{D06E75A8-357E-43FF-BB71-9220563B4FF1}" name="vom_cost_Output1"/>
+    <tableColumn id="23" xr3:uid="{07DC8CB6-C272-41D4-80ED-FF8256CC8FCE}" name="vom_cost_Output2"/>
+    <tableColumn id="15" xr3:uid="{950CF4AC-5CFC-4BCA-8A22-8C86AB3DB733}" name="minimum_op_point_Input1"/>
+    <tableColumn id="14" xr3:uid="{ABF46C45-CFC5-4F2E-AE43-5546362399A3}" name="minimum_op_point_Input2"/>
+    <tableColumn id="7" xr3:uid="{A161C114-3468-49D8-8F0C-42BFB654C6E0}" name="minimum_op_point_Output1"/>
+    <tableColumn id="6" xr3:uid="{4E34AA21-6766-42EA-A651-4C70A54CFE6B}" name="minimum_op_point_Output2"/>
+    <tableColumn id="38" xr3:uid="{98E9C0E9-88C9-4D30-849B-984AB1D75A7D}" name="resolution_output" dataDxfId="3"/>
+    <tableColumn id="39" xr3:uid="{03AC4D02-73C3-4D48-821E-72DFEECBD86E}" name="demand" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:AB5" totalsRowShown="0">
-  <autoFilter ref="A1:AB5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
-    <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Object_type"/>
-    <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input1"/>
-    <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Input2"/>
-    <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output1"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Output2" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Connection_type"/>
-    <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_existing"/>
-    <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input1_max"/>
-    <tableColumn id="7" xr3:uid="{E7E4A800-7F3E-4BF9-A884-F3BDD87E4621}" name="Cap_Input2_existing"/>
-    <tableColumn id="16" xr3:uid="{8893BE03-F801-4096-BA71-49D3B6176542}" name="Cap_Input2_max"/>
-    <tableColumn id="17" xr3:uid="{9DC965EA-6654-4828-B29B-097368A09D75}" name="Cap_Output1_existing"/>
-    <tableColumn id="19" xr3:uid="{CB576510-488A-48D1-9EBF-E417CAAAB7E4}" name="Cap_Output1_max"/>
-    <tableColumn id="20" xr3:uid="{5176DB25-AD8B-43E3-AEAF-7F27C99BEFB0}" name="Cap_Output2_existing"/>
-    <tableColumn id="8" xr3:uid="{5E25F56C-3E8C-4A4F-ACEB-CDBC45CA165F}" name="Cap_Output2_max"/>
-    <tableColumn id="18" xr3:uid="{5D07405F-AE18-4D9F-96A6-B56AE42485A2}" name="Efficency"/>
-    <tableColumn id="9" xr3:uid="{3138804A-F699-4287-89C7-DE76BAD06195}" name="Relation_In_In"/>
-    <tableColumn id="10" xr3:uid="{AE158189-8F74-4D1A-BE7F-20B56DC1FCA0}" name="Relation_In_Out"/>
-    <tableColumn id="23" xr3:uid="{C3B5D3DD-6B9E-4750-8098-2BDCA6D4F76B}" name="Relation_Out_Out"/>
-    <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Relation_Out_In"/>
-    <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="Cost_invest"/>
-    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="fom_cost"/>
-    <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input1"/>
-    <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Input2"/>
-    <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output1"/>
-    <tableColumn id="26" xr3:uid="{BBB71EDD-0EC0-477F-903A-3BF251C590FC}" name="vom_cost_Output2"/>
-    <tableColumn id="27" xr3:uid="{65A6FC97-CBF5-4192-8668-F1903C17C1F5}" name="connection_investment_tech_lifetime"/>
-    <tableColumn id="28" xr3:uid="{6C87744B-3FF9-44BB-9394-82EE6DD0EE4E}" name="number_of_connections"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3CFFDFB0-142A-401E-88DC-36CE97F43F11}" name="Table138" displayName="Table138" ref="A1:AA5" totalsRowShown="0">
+  <autoFilter ref="A1:AA5" xr:uid="{3CFFDFB0-142A-401E-88DC-36CE97F43F11}"/>
+  <tableColumns count="27">
+    <tableColumn id="1" xr3:uid="{7224490A-92A9-4DB7-8F18-50B916450AED}" name="Connection"/>
+    <tableColumn id="26" xr3:uid="{AB2D4FE6-9B42-499A-9949-C00E98104D63}" name="Object_type"/>
+    <tableColumn id="2" xr3:uid="{748008A0-5B3A-4243-80E0-114D78BB66C8}" name="Input1"/>
+    <tableColumn id="3" xr3:uid="{E30D8E2D-EEF4-4BF1-94CB-FFEE34536A1F}" name="Input2"/>
+    <tableColumn id="4" xr3:uid="{D52FC770-9E65-420D-9FFC-FA21A8D93B3B}" name="Output1"/>
+    <tableColumn id="5" xr3:uid="{B64E5B50-6A85-4A5C-9781-6A9F33894040}" name="Output2"/>
+    <tableColumn id="22" xr3:uid="{1BB07178-678F-4545-9041-9A5C7D5846C0}" name="Connection_type" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C2C375E4-A8ED-4591-9F3C-B0312491F92E}" name="Cap_Input1_existing"/>
+    <tableColumn id="15" xr3:uid="{4D2B916D-D300-434A-8EC1-8C99CC1C7668}" name="Cap_Input1_max"/>
+    <tableColumn id="14" xr3:uid="{76BC126E-6B1E-4266-9DB1-BF720DBE9AEB}" name="Cap_Input2_existing"/>
+    <tableColumn id="7" xr3:uid="{CE74ADE8-2E32-4FF2-84A0-700E97B22289}" name="Cap_Input2_max"/>
+    <tableColumn id="16" xr3:uid="{29D53571-EDB3-44AB-876C-F29737F48B07}" name="Cap_Output1_existing"/>
+    <tableColumn id="17" xr3:uid="{07F875AF-C538-4C2F-B89D-7885C5EE1815}" name="Cap_Output1_max"/>
+    <tableColumn id="19" xr3:uid="{61A50197-1EFA-4D58-917B-313C114A8BA9}" name="Cap_Output2_existing"/>
+    <tableColumn id="20" xr3:uid="{E614D03C-664F-482D-B3D9-AA71DAD527CC}" name="Cap_Output2_max"/>
+    <tableColumn id="8" xr3:uid="{9FAA31F9-849A-4634-A130-EEC3FF78C7CE}" name="Efficency"/>
+    <tableColumn id="18" xr3:uid="{A152B25D-0C2E-4007-8B84-C8E6EE3DE5E0}" name="Relation_In_In"/>
+    <tableColumn id="9" xr3:uid="{28CA02C0-27EC-419F-BAA6-5399D591CD3D}" name="Relation_In_Out"/>
+    <tableColumn id="10" xr3:uid="{F0A4FFB0-4AEF-43C4-BE95-3B66F391CBA2}" name="Relation_Out_Out"/>
+    <tableColumn id="23" xr3:uid="{45F57C34-107F-494B-80C2-FF5656CDDCD6}" name="Relation_Out_In"/>
+    <tableColumn id="12" xr3:uid="{67D49085-32DC-479A-9AAF-AA109539234D}" name="fom_cost"/>
+    <tableColumn id="13" xr3:uid="{28CFCB19-E44E-4BB4-8E0A-37D50D3CCE56}" name="vom_cost_Input1"/>
+    <tableColumn id="21" xr3:uid="{0AA44873-6A86-4A91-8056-F3F2542D8290}" name="vom_cost_Input2"/>
+    <tableColumn id="24" xr3:uid="{6468F7C1-5EAA-4265-B109-2B6B92B69E6B}" name="vom_cost_Output1"/>
+    <tableColumn id="25" xr3:uid="{7CA03FEF-C526-4FC4-A995-E18EEBD66423}" name="vom_cost_Output2"/>
+    <tableColumn id="29" xr3:uid="{8B68CA3A-C71C-424D-9FE6-541BD8B756E2}" name="connection_investment_tech_lifetime" dataDxfId="0"/>
+    <tableColumn id="30" xr3:uid="{3DFFCE40-F2C4-4E41-A306-FD9531E7482E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:N5" totalsRowShown="0">
-  <autoFilter ref="A1:N5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:L5" totalsRowShown="0">
+  <autoFilter ref="A1:L5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="Object_type"/>
     <tableColumn id="6" xr3:uid="{FA5F8582-61FC-4A96-9E8D-E08E92F1962D}" name="value_before"/>
     <tableColumn id="5" xr3:uid="{58DBFD58-A0D2-4B31-B639-19B1628ABAC8}" name="value_start"/>
@@ -624,9 +549,7 @@
     <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="Cost_invest"/>
     <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="fom_cost"/>
     <tableColumn id="8" xr3:uid="{D3E26ECE-7BB7-42B8-829D-538BD4CDBDB6}" name="vom_cost"/>
-    <tableColumn id="9" xr3:uid="{0A1D8BBC-00AA-4BE2-AE05-790AC3DC8C47}" name="storage_investment_tech_lifetime"/>
-    <tableColumn id="10" xr3:uid="{2C02AE75-18E1-43C0-BD7D-2A33CD6D2344}" name="number_of_storages"/>
-    <tableColumn id="14" xr3:uid="{B6B58E65-7932-4722-B6A3-B26FE39DEC3E}" name="storage_investment_cost"/>
+    <tableColumn id="9" xr3:uid="{8FAF8F23-6AED-4FFE-88CE-FC2372BEB57A}" name="initial_storages_invested"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -939,41 +862,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AQ6"/>
+  <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="4" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.08984375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="20.08984375" customWidth="1"/>
     <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" hidden="1" customWidth="1"/>
-    <col min="14" max="22" width="10.54296875" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="12.7265625" customWidth="1"/>
-    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" customWidth="1"/>
-    <col min="30" max="30" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="27" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -988,302 +919,229 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2">
+        <v>1.29</v>
+      </c>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3">
+        <v>0.75</v>
+      </c>
+      <c r="S3">
+        <v>5.8500000000000002E-3</v>
+      </c>
+      <c r="U3">
+        <v>1.76</v>
+      </c>
+      <c r="X3">
+        <v>4.34</v>
+      </c>
+      <c r="AA3">
+        <v>1.4865951742627345E-3</v>
+      </c>
+      <c r="AD3">
+        <v>0.02</v>
+      </c>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2">
-        <v>304</v>
-      </c>
-      <c r="L2">
-        <v>304</v>
-      </c>
-      <c r="AB2" t="e">
-        <f>[1]!Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AD2">
-        <v>1.29</v>
-      </c>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="4"/>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4">
+        <v>7.2437800000000002E-4</v>
+      </c>
+      <c r="T4">
+        <v>0.99</v>
+      </c>
+      <c r="X4">
+        <v>0.11929223744292237</v>
+      </c>
+      <c r="AA4">
+        <v>1.4865951742627345E-3</v>
+      </c>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="2"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3">
-        <v>52</v>
-      </c>
-      <c r="H3">
-        <v>52</v>
-      </c>
-      <c r="O3">
-        <v>0.75</v>
-      </c>
-      <c r="Y3">
-        <v>5.8500000000000002E-3</v>
-      </c>
-      <c r="AA3">
-        <v>1.76</v>
-      </c>
-      <c r="AD3">
-        <v>4.34</v>
-      </c>
-      <c r="AG3">
-        <v>1.4865951742627345E-3</v>
-      </c>
-      <c r="AJ3">
-        <v>0.02</v>
-      </c>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="4"/>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="Y4">
-        <v>7.2437800000000002E-4</v>
-      </c>
-      <c r="Z4">
-        <v>0.99</v>
-      </c>
-      <c r="AD4">
-        <v>0.11929223744292237</v>
-      </c>
-      <c r="AG4">
-        <v>1.4865951742627345E-3</v>
-      </c>
-      <c r="AK4">
-        <v>0.1</v>
-      </c>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
-      <c r="AN4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AP4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="4"/>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB5" t="e">
-        <f>[1]!Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" t="s">
-        <v>104</v>
-      </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB6" t="e">
-        <f>[1]!Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
-        <v>#REF!</v>
+        <v>80</v>
+      </c>
+      <c r="G6">
+        <v>0.7</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>20.192799999999998</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL4" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2:AH6" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1298,7 +1156,7 @@
           <x14:formula1>
             <xm:f>DropDown!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
+          <xm:sqref>B4:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1308,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1320,13 +1178,13 @@
     <col min="4" max="5" width="9.81640625" customWidth="1"/>
     <col min="6" max="6" width="17.08984375" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
     <col min="9" max="9" width="15.36328125" customWidth="1"/>
-    <col min="10" max="10" width="1.7265625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.36328125" customWidth="1"/>
-    <col min="12" max="12" width="19" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="15.36328125" customWidth="1"/>
-    <col min="14" max="14" width="19" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="10.54296875" customWidth="1"/>
     <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1"/>
@@ -1337,12 +1195,12 @@
     <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1357,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -1387,25 +1245,25 @@
         <v>5</v>
       </c>
       <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
       <c r="T1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="V1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
         <v>30</v>
-      </c>
-      <c r="W1" t="s">
-        <v>34</v>
       </c>
       <c r="X1" t="s">
         <v>31</v>
@@ -1414,36 +1272,33 @@
         <v>32</v>
       </c>
       <c r="Z1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="AA1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1475,34 +1330,34 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="AA2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB2">
+      <c r="Z2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1528,37 +1383,37 @@
       <c r="T3">
         <v>0.88</v>
       </c>
-      <c r="V3">
+      <c r="U3">
         <v>7.2835616438356163E-2</v>
       </c>
-      <c r="AA3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB3">
+      <c r="Z3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
         <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1578,28 +1433,28 @@
       <c r="N4">
         <v>1000</v>
       </c>
-      <c r="AA4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB4">
+      <c r="Z4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>89</v>
       </c>
       <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" t="s">
-        <v>91</v>
-      </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1616,10 +1471,10 @@
       <c r="T5">
         <v>1</v>
       </c>
-      <c r="AA5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB5">
+      <c r="Z5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA5">
         <v>1</v>
       </c>
     </row>
@@ -1634,76 +1489,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1718,24 +1568,18 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2">
+        <v>53</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>0.121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1744,12 +1588,9 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3">
+        <v>53</v>
+      </c>
+      <c r="L3">
         <v>0</v>
       </c>
     </row>
@@ -1772,84 +1613,87 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated numbers in model data bases
Rows that need attention are highlighted in yellow.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2E42E8E-BC70-4891-85BD-0F04F6277FFF}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AD48935-E225-45FD-A842-9F4D1EE3F5E0}"/>
   <bookViews>
-    <workbookView xWindow="-20835" yWindow="-19260" windowWidth="22860" windowHeight="18315" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
   <si>
     <t>Unit</t>
   </si>
@@ -319,9 +319,6 @@
   </si>
   <si>
     <t>steam</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
   <si>
     <t>steam_plant</t>
@@ -388,12 +385,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -408,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -416,11 +419,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -438,9 +445,6 @@
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -454,10 +458,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}" name="Table16" displayName="Table16" ref="A1:AI6" totalsRowShown="0">
-  <autoFilter ref="A1:AI6" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}"/>
-  <tableColumns count="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}" name="Table16" displayName="Table16" ref="A1:AH6" totalsRowShown="0">
+  <autoFilter ref="A1:AH6" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{7D298EC1-7302-405B-8F92-0542D7D7F128}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{DCBF9D29-057B-4317-8290-D82D5B7920ED}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{D57D27A7-B5BF-44EE-97E6-A45E663C9B11}" name="Input1"/>
@@ -479,7 +487,6 @@
     <tableColumn id="9" xr3:uid="{7094586D-F569-42E6-9659-BFA01BFADAC8}" name="Relation_In_In"/>
     <tableColumn id="20" xr3:uid="{147C72B7-620D-4714-87E9-E7CB6F571574}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{E3C2CD93-F547-4D58-8A39-A1C9F02F97A8}" name="Relation_Out_Out"/>
-    <tableColumn id="11" xr3:uid="{2EC6318E-BECE-45C0-8327-D7AFF840871E}" name="Cost_invest"/>
     <tableColumn id="25" xr3:uid="{9F049A47-0213-4397-848B-1EF1B3A45E7A}" name="units_on_cost"/>
     <tableColumn id="12" xr3:uid="{C4243E50-4545-43FB-A14B-E5CD366C40F9}" name="fom_cost"/>
     <tableColumn id="24" xr3:uid="{2887EEF0-F5F4-42D9-AF95-2AE9F59DB77A}" name="vom_cost"/>
@@ -491,8 +498,8 @@
     <tableColumn id="14" xr3:uid="{ABF46C45-CFC5-4F2E-AE43-5546362399A3}" name="minimum_op_point_Input2"/>
     <tableColumn id="7" xr3:uid="{A161C114-3468-49D8-8F0C-42BFB654C6E0}" name="minimum_op_point_Output1"/>
     <tableColumn id="6" xr3:uid="{4E34AA21-6766-42EA-A651-4C70A54CFE6B}" name="minimum_op_point_Output2"/>
-    <tableColumn id="38" xr3:uid="{98E9C0E9-88C9-4D30-849B-984AB1D75A7D}" name="resolution_output" dataDxfId="3"/>
-    <tableColumn id="39" xr3:uid="{03AC4D02-73C3-4D48-821E-72DFEECBD86E}" name="demand" dataDxfId="2"/>
+    <tableColumn id="38" xr3:uid="{98E9C0E9-88C9-4D30-849B-984AB1D75A7D}" name="resolution_output" dataDxfId="4"/>
+    <tableColumn id="39" xr3:uid="{03AC4D02-73C3-4D48-821E-72DFEECBD86E}" name="demand" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -508,7 +515,7 @@
     <tableColumn id="3" xr3:uid="{E30D8E2D-EEF4-4BF1-94CB-FFEE34536A1F}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{D52FC770-9E65-420D-9FFC-FA21A8D93B3B}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{B64E5B50-6A85-4A5C-9781-6A9F33894040}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{1BB07178-678F-4545-9041-9A5C7D5846C0}" name="Connection_type" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{1BB07178-678F-4545-9041-9A5C7D5846C0}" name="Connection_type" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{C2C375E4-A8ED-4591-9F3C-B0312491F92E}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{4D2B916D-D300-434A-8EC1-8C99CC1C7668}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{76BC126E-6B1E-4266-9DB1-BF720DBE9AEB}" name="Cap_Input2_existing"/>
@@ -527,7 +534,7 @@
     <tableColumn id="21" xr3:uid="{0AA44873-6A86-4A91-8056-F3F2542D8290}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{6468F7C1-5EAA-4265-B109-2B6B92B69E6B}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{7CA03FEF-C526-4FC4-A995-E18EEBD66423}" name="vom_cost_Output2"/>
-    <tableColumn id="29" xr3:uid="{8B68CA3A-C71C-424D-9FE6-541BD8B756E2}" name="connection_investment_tech_lifetime" dataDxfId="0"/>
+    <tableColumn id="29" xr3:uid="{8B68CA3A-C71C-424D-9FE6-541BD8B756E2}" name="connection_investment_tech_lifetime" dataDxfId="1"/>
     <tableColumn id="30" xr3:uid="{3DFFCE40-F2C4-4E41-A306-FD9531E7482E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -538,7 +545,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:L5" totalsRowShown="0">
   <autoFilter ref="A1:L5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="Object_type"/>
     <tableColumn id="6" xr3:uid="{FA5F8582-61FC-4A96-9E8D-E08E92F1962D}" name="value_before"/>
     <tableColumn id="5" xr3:uid="{58DBFD58-A0D2-4B31-B639-19B1628ABAC8}" name="value_start"/>
@@ -862,11 +869,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -887,19 +892,18 @@
     <col min="19" max="19" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="27" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="27" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -964,49 +968,46 @@
         <v>18</v>
       </c>
       <c r="V1" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="W1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="X1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="Z1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AB1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AC1" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="AD1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AE1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AF1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AG1" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="AH1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1016,13 +1017,10 @@
       <c r="E2" t="s">
         <v>76</v>
       </c>
-      <c r="X2">
-        <v>1.29</v>
-      </c>
+      <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1050,21 +1048,21 @@
       <c r="U3">
         <v>1.76</v>
       </c>
-      <c r="X3">
+      <c r="W3">
         <v>4.34</v>
       </c>
-      <c r="AA3">
-        <v>1.4865951742627345E-3</v>
-      </c>
-      <c r="AD3">
+      <c r="Y3">
+        <v>1.4865950000000001E-3</v>
+      </c>
+      <c r="AC3">
         <v>0.02</v>
       </c>
+      <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -1084,18 +1082,18 @@
       <c r="T4">
         <v>0.99</v>
       </c>
-      <c r="X4">
-        <v>0.11929223744292237</v>
-      </c>
-      <c r="AA4">
-        <v>1.4865951742627345E-3</v>
-      </c>
+      <c r="W4">
+        <v>0.11929223999999999</v>
+      </c>
+      <c r="Z4">
+        <v>1.4865950000000001E-3</v>
+      </c>
+      <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>91</v>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
@@ -1104,14 +1102,14 @@
         <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="2"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="2"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
@@ -1120,28 +1118,21 @@
         <v>79</v>
       </c>
       <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
         <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>93</v>
       </c>
       <c r="F6" t="s">
         <v>80</v>
       </c>
-      <c r="G6">
-        <v>0.7</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>20.192799999999998</v>
-      </c>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2:AH6" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG6" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1168,16 +1159,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" customWidth="1"/>
-    <col min="4" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="17.08984375" customWidth="1"/>
+    <col min="7" max="7" width="33.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.453125" customWidth="1"/>
     <col min="9" max="9" width="15.36328125" customWidth="1"/>
     <col min="10" max="10" width="20.7265625" bestFit="1" customWidth="1"/>
@@ -1275,18 +1264,18 @@
         <v>44</v>
       </c>
       <c r="AA1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
         <v>76</v>
@@ -1295,7 +1284,7 @@
         <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
         <v>56</v>
@@ -1339,7 +1328,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -1348,10 +1337,10 @@
         <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
         <v>79</v>
@@ -1394,23 +1383,23 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>95</v>
+      <c r="A4" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
         <v>59</v>
@@ -1442,7 +1431,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -1451,7 +1440,7 @@
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
         <v>59</v>
@@ -1491,9 +1480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1545,12 +1532,12 @@
         <v>28</v>
       </c>
       <c r="L1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
@@ -1575,8 +1562,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>96</v>
+      <c r="A3" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
update input templates in excel
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\ammonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AD48935-E225-45FD-A842-9F4D1EE3F5E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBB7DFD-AC4C-46DD-9F2F-8D2E9921244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="99">
   <si>
     <t>Unit</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>initial_storages_invested</t>
+  </si>
+  <si>
+    <t>nh3_synthesis_power</t>
+  </si>
+  <si>
+    <t>nh3_raw</t>
   </si>
 </sst>
 </file>
@@ -458,13 +464,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}" name="Table16" displayName="Table16" ref="A1:AH6" totalsRowShown="0">
-  <autoFilter ref="A1:AH6" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}" name="Table16" displayName="Table16" ref="A1:AH7" totalsRowShown="0">
+  <autoFilter ref="A1:AH7" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}"/>
   <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{7D298EC1-7302-405B-8F92-0542D7D7F128}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{DCBF9D29-057B-4317-8290-D82D5B7920ED}" name="Object_type"/>
@@ -869,13 +871,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.453125" customWidth="1"/>
@@ -1121,18 +1125,34 @@
         <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
         <v>80</v>
       </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="2"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG6" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG7" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added a power storage option
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{1CBB7DFD-AC4C-46DD-9F2F-8D2E9921244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C654723A-E987-43DA-B4A6-B4255B1F7934}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1CBB7DFD-AC4C-46DD-9F2F-8D2E9921244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8C008F-8E63-4C91-91D4-A400B6AF9FB9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -462,6 +462,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1201,6 +1205,7 @@
     <col min="20" max="20" width="12.7265625" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Took out hard-coded values in input prep
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1CBB7DFD-AC4C-46DD-9F2F-8D2E9921244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8C008F-8E63-4C91-91D4-A400B6AF9FB9}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{1CBB7DFD-AC4C-46DD-9F2F-8D2E9921244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C9E8525-77FA-4E99-B62D-FE73ECA160EE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
   <si>
     <t>Unit</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Power_storage</t>
+  </si>
+  <si>
+    <t>initial_units_on</t>
   </si>
 </sst>
 </file>
@@ -469,9 +472,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}" name="Table16" displayName="Table16" ref="A1:AH7" totalsRowShown="0">
-  <autoFilter ref="A1:AH7" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}"/>
-  <tableColumns count="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}" name="Table16" displayName="Table16" ref="A1:AI7" totalsRowShown="0">
+  <autoFilter ref="A1:AI7" xr:uid="{025174FC-A356-4B24-981E-7C11DD30745B}"/>
+  <tableColumns count="35">
     <tableColumn id="1" xr3:uid="{7D298EC1-7302-405B-8F92-0542D7D7F128}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{DCBF9D29-057B-4317-8290-D82D5B7920ED}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{D57D27A7-B5BF-44EE-97E6-A45E663C9B11}" name="Input1"/>
@@ -506,6 +509,7 @@
     <tableColumn id="6" xr3:uid="{4E34AA21-6766-42EA-A651-4C70A54CFE6B}" name="minimum_op_point_Output2"/>
     <tableColumn id="38" xr3:uid="{98E9C0E9-88C9-4D30-849B-984AB1D75A7D}" name="resolution_output" dataDxfId="4"/>
     <tableColumn id="39" xr3:uid="{03AC4D02-73C3-4D48-821E-72DFEECBD86E}" name="demand" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{785FBF70-6702-4C9F-842A-5E88B1A36BB2}" name="initial_units_on"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -874,9 +878,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -906,9 +910,10 @@
     <col min="31" max="32" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1011,8 +1016,11 @@
       <c r="AH1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AI1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1025,7 +1033,7 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1065,7 +1073,7 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -1096,7 +1104,7 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>89</v>
       </c>
@@ -1112,7 +1120,7 @@
       <c r="AG5" s="1"/>
       <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>92</v>
       </c>
@@ -1134,7 +1142,7 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1148,7 +1156,9 @@
         <v>91</v>
       </c>
       <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
+      <c r="AH7" s="1">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1180,9 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
High - Low Heat
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{1CBB7DFD-AC4C-46DD-9F2F-8D2E9921244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C9E8525-77FA-4E99-B62D-FE73ECA160EE}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{1CBB7DFD-AC4C-46DD-9F2F-8D2E9921244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6323901D-E487-40A2-AA7C-6363967171B8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="555" yWindow="-17445" windowWidth="14400" windowHeight="8265" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="105">
   <si>
     <t>Unit</t>
   </si>
@@ -312,9 +312,6 @@
     <t>h2</t>
   </si>
   <si>
-    <t>heat</t>
-  </si>
-  <si>
     <t>steam</t>
   </si>
   <si>
@@ -373,6 +370,24 @@
   </si>
   <si>
     <t>initial_units_on</t>
+  </si>
+  <si>
+    <t>heat_low</t>
+  </si>
+  <si>
+    <t>heat_high</t>
+  </si>
+  <si>
+    <t>heat_split</t>
+  </si>
+  <si>
+    <t>Auxilliary</t>
+  </si>
+  <si>
+    <t>internal_heat</t>
+  </si>
+  <si>
+    <t>Auxiliary</t>
   </si>
 </sst>
 </file>
@@ -572,8 +587,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F60E0718-CF3D-46DE-ABAE-954431E3B623}" name="Table4" displayName="Table4" ref="A1:A16" totalsRowShown="0">
-  <autoFilter ref="A1:A16" xr:uid="{F60E0718-CF3D-46DE-ABAE-954431E3B623}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F60E0718-CF3D-46DE-ABAE-954431E3B623}" name="Table4" displayName="Table4" ref="A1:A17" totalsRowShown="0">
+  <autoFilter ref="A1:A17" xr:uid="{F60E0718-CF3D-46DE-ABAE-954431E3B623}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{92FD8766-2E9E-48CC-B065-131067C79BF9}" name="object_type"/>
   </tableColumns>
@@ -878,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -913,7 +928,7 @@
     <col min="35" max="35" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1017,10 +1032,10 @@
         <v>47</v>
       </c>
       <c r="AI1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1033,7 +1048,7 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="G3">
         <v>0.75</v>
@@ -1073,9 +1088,9 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -1087,7 +1102,7 @@
         <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S4">
         <v>7.2437800000000002E-4</v>
@@ -1104,9 +1119,9 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
         <v>66</v>
@@ -1115,14 +1130,14 @@
         <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>67</v>
@@ -1131,39 +1146,61 @@
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1">
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="U8">
+        <v>0.4</v>
+      </c>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG7" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG7 AI8" xr:uid="{ED867B80-C728-4873-8D4D-BAB1E8AB7F30}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1178,7 +1215,7 @@
           <x14:formula1>
             <xm:f>DropDown!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B4:B1048576</xm:sqref>
+          <xm:sqref>B4:B7 B9:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1296,18 +1333,18 @@
         <v>43</v>
       </c>
       <c r="AA1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>75</v>
@@ -1316,7 +1353,7 @@
         <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
         <v>55</v>
@@ -1360,7 +1397,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -1369,10 +1406,10 @@
         <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
         <v>78</v>
@@ -1416,22 +1453,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
         <v>58</v>
@@ -1463,16 +1500,16 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
         <v>58</v>
@@ -1560,12 +1597,12 @@
         <v>27</v>
       </c>
       <c r="K1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -1591,7 +1628,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
@@ -1625,11 +1662,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F682EA3-CCEB-45E2-AC25-979810840C6C}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1713,7 +1748,12 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>